<commit_message>
Revert "only four distractors"
This reverts commit 751abc92
</commit_message>
<xml_diff>
--- a/new_bci_framework/paradigm/p300_paradigm/res/only_stim_words.xlsx
+++ b/new_bci_framework/paradigm/p300_paradigm/res/only_stim_words.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\python\bci4als-2022-python\new_bci_framework\paradigm\p300_paradigm\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\python\bci4als-2022-python\new_bci_framework\paradigm\p300_paradigm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8254651-5743-4F2F-9016-C8BE11665857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC731A42-5DFF-4ED7-AC2F-F02498EC4810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="8340" windowWidth="19365" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>word</t>
   </si>
@@ -186,43 +186,52 @@
     <t>שער</t>
   </si>
   <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\NOhebYardenSHORT.wav</t>
-  </si>
-  <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\YEShebYardenSHORT.wav</t>
-  </si>
-  <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\PinkNoise.wav</t>
-  </si>
-  <si>
     <t>came</t>
   </si>
   <si>
     <t>hot</t>
   </si>
   <si>
+    <t>indicator</t>
+  </si>
+  <si>
+    <t>candle</t>
+  </si>
+  <si>
+    <t>רנ</t>
+  </si>
+  <si>
+    <t>דמ</t>
+  </si>
+  <si>
     <t>םח</t>
   </si>
   <si>
     <t>אב</t>
   </si>
   <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\CAMEhebYarden.wav</t>
-  </si>
-  <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\HOThebYarden.wav</t>
-  </si>
-  <si>
     <t>target</t>
   </si>
   <si>
-    <t>minister</t>
-  </si>
-  <si>
-    <t>רש</t>
-  </si>
-  <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\MINISTERhebYarden.wav</t>
+    <t>YEShebYardenSHORT.wav</t>
+  </si>
+  <si>
+    <t>NOhebYardenSHORT.wav</t>
+  </si>
+  <si>
+    <t>PinkNoise.wav</t>
+  </si>
+  <si>
+    <t>CAMEhebYarden.wav</t>
+  </si>
+  <si>
+    <t>HOThebYarden.wav</t>
+  </si>
+  <si>
+    <t>INDICATORhebYarden.wav</t>
+  </si>
+  <si>
+    <t>CANDLEhebYarden.wav</t>
   </si>
 </sst>
 </file>
@@ -617,11 +626,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -645,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -659,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -676,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -693,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -701,16 +710,16 @@
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -718,16 +727,16 @@
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -735,18 +744,35 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2">
         <v>0</v>
       </c>
     </row>
@@ -763,6 +789,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F5CAB0486A994CA2C3B13E059EF2AE" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8645ec4a60d0c8c7009d2d6675847a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="636d7205651659ec4fcda0bcbde9384b">
     <xsd:element name="properties">
@@ -876,12 +908,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -892,6 +918,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -907,21 +948,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
   <ds:schemaRefs>

</xml_diff>